<commit_message>
complete running version with only minor discrepancies. also first try with travis.yml
</commit_message>
<xml_diff>
--- a/data/snyder_et_al_feature_classes.xlsx
+++ b/data/snyder_et_al_feature_classes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmackey/Google Drive/Documents/Research Projects/su2c/survival-analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdml/Desktop/multifactorial-immune-response/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="94">
   <si>
     <t>#Feature name</t>
   </si>
@@ -294,21 +294,6 @@
   </si>
   <si>
     <t>Unique TIL clones in C(cnt)</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>I-R</t>
-  </si>
-  <si>
-    <t>Invasive</t>
   </si>
   <si>
     <t>NExpanded Clones that were TILs A-&gt;B</t>
@@ -641,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,7 +637,7 @@
     <col min="1" max="1" width="62.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -665,11 +650,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -682,11 +664,8 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -699,11 +678,8 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -716,11 +692,8 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -733,11 +706,8 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -750,11 +720,8 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -767,11 +734,8 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -784,11 +748,8 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -801,11 +762,8 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -818,11 +776,8 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -835,11 +790,8 @@
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -852,11 +804,8 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -869,11 +818,8 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -886,11 +832,8 @@
       <c r="D14" t="b">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -903,11 +846,8 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -920,11 +860,8 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -937,11 +874,8 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -954,11 +888,8 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -971,11 +902,8 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -988,11 +916,8 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1005,11 +930,8 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1022,11 +944,8 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1039,13 +958,10 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -1056,11 +972,8 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="E24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1073,11 +986,8 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="E25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1090,11 +1000,8 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1107,11 +1014,8 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
-      <c r="E27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1124,11 +1028,8 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1141,11 +1042,8 @@
       <c r="D29" t="b">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1158,11 +1056,8 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1175,11 +1070,8 @@
       <c r="D31" t="b">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1192,11 +1084,8 @@
       <c r="D32" t="b">
         <v>0</v>
       </c>
-      <c r="E32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1209,11 +1098,8 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
-      <c r="E33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1226,11 +1112,8 @@
       <c r="D34" t="b">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1243,11 +1126,8 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1260,11 +1140,8 @@
       <c r="D36" t="b">
         <v>1</v>
       </c>
-      <c r="E36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1277,11 +1154,8 @@
       <c r="D37" t="b">
         <v>1</v>
       </c>
-      <c r="E37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1294,11 +1168,8 @@
       <c r="D38" t="b">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1311,11 +1182,8 @@
       <c r="D39" t="b">
         <v>0</v>
       </c>
-      <c r="E39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1328,11 +1196,8 @@
       <c r="D40" t="b">
         <v>0</v>
       </c>
-      <c r="E40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1345,11 +1210,8 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
-      <c r="E41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1362,11 +1224,8 @@
       <c r="D42" t="b">
         <v>0</v>
       </c>
-      <c r="E42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1379,11 +1238,8 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1396,11 +1252,8 @@
       <c r="D44" t="b">
         <v>0</v>
       </c>
-      <c r="E44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -1413,11 +1266,8 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
-      <c r="E45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1430,11 +1280,8 @@
       <c r="D46" t="b">
         <v>0</v>
       </c>
-      <c r="E46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -1447,11 +1294,8 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
-      <c r="E47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -1464,11 +1308,8 @@
       <c r="D48" t="b">
         <v>0</v>
       </c>
-      <c r="E48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1481,11 +1322,8 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
-      <c r="E49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -1498,11 +1336,8 @@
       <c r="D50" t="b">
         <v>0</v>
       </c>
-      <c r="E50" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -1515,11 +1350,8 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
-      <c r="E51" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1532,11 +1364,8 @@
       <c r="D52" t="b">
         <v>0</v>
       </c>
-      <c r="E52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -1549,11 +1378,8 @@
       <c r="D53" t="b">
         <v>0</v>
       </c>
-      <c r="E53" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -1566,11 +1392,8 @@
       <c r="D54" t="b">
         <v>0</v>
       </c>
-      <c r="E54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -1583,11 +1406,8 @@
       <c r="D55" t="b">
         <v>0</v>
       </c>
-      <c r="E55" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -1600,11 +1420,8 @@
       <c r="D56" t="b">
         <v>0</v>
       </c>
-      <c r="E56" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1617,11 +1434,8 @@
       <c r="D57" t="b">
         <v>0</v>
       </c>
-      <c r="E57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -1634,11 +1448,8 @@
       <c r="D58" t="b">
         <v>0</v>
       </c>
-      <c r="E58" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -1651,11 +1462,8 @@
       <c r="D59" t="b">
         <v>0</v>
       </c>
-      <c r="E59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -1668,11 +1476,8 @@
       <c r="D60" t="b">
         <v>0</v>
       </c>
-      <c r="E60" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -1685,11 +1490,8 @@
       <c r="D61" t="b">
         <v>0</v>
       </c>
-      <c r="E61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -1702,11 +1504,8 @@
       <c r="D62" t="b">
         <v>0</v>
       </c>
-      <c r="E62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -1719,11 +1518,8 @@
       <c r="D63" t="b">
         <v>0</v>
       </c>
-      <c r="E63" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -1736,11 +1532,8 @@
       <c r="D64" t="b">
         <v>0</v>
       </c>
-      <c r="E64" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -1753,11 +1546,8 @@
       <c r="D65" t="b">
         <v>0</v>
       </c>
-      <c r="E65" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -1770,11 +1560,8 @@
       <c r="D66" t="b">
         <v>0</v>
       </c>
-      <c r="E66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -1787,11 +1574,8 @@
       <c r="D67" t="b">
         <v>0</v>
       </c>
-      <c r="E67" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -1804,11 +1588,8 @@
       <c r="D68" t="b">
         <v>0</v>
       </c>
-      <c r="E68" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -1821,11 +1602,8 @@
       <c r="D69" t="b">
         <v>0</v>
       </c>
-      <c r="E69" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -1838,11 +1616,8 @@
       <c r="D70" t="b">
         <v>0</v>
       </c>
-      <c r="E70" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -1855,11 +1630,8 @@
       <c r="D71" t="b">
         <v>0</v>
       </c>
-      <c r="E71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -1872,11 +1644,8 @@
       <c r="D72" t="b">
         <v>0</v>
       </c>
-      <c r="E72" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -1889,11 +1658,8 @@
       <c r="D73" t="b">
         <v>0</v>
       </c>
-      <c r="E73" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -1906,11 +1672,8 @@
       <c r="D74" t="b">
         <v>0</v>
       </c>
-      <c r="E74" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -1923,11 +1686,8 @@
       <c r="D75" t="b">
         <v>0</v>
       </c>
-      <c r="E75" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -1940,13 +1700,10 @@
       <c r="D76" t="b">
         <v>0</v>
       </c>
-      <c r="E76" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
         <v>84</v>
@@ -1957,13 +1714,10 @@
       <c r="D77" t="b">
         <v>0</v>
       </c>
-      <c r="E77" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B78" t="s">
         <v>84</v>
@@ -1974,11 +1728,8 @@
       <c r="D78" t="b">
         <v>0</v>
       </c>
-      <c r="E78" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -1991,13 +1742,10 @@
       <c r="D79" t="b">
         <v>0</v>
       </c>
-      <c r="E79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
@@ -2008,13 +1756,10 @@
       <c r="D80" t="b">
         <v>0</v>
       </c>
-      <c r="E80" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>97</v>
       </c>
       <c r="B81" t="s">
         <v>84</v>
@@ -2025,11 +1770,8 @@
       <c r="D81" t="b">
         <v>0</v>
       </c>
-      <c r="E81" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2041,9 +1783,6 @@
       </c>
       <c r="D82" t="b">
         <v>0</v>
-      </c>
-      <c r="E82" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>